<commit_message>
del 2 files DB
</commit_message>
<xml_diff>
--- a/server/src/api/INPUT_/NaturaLP_ANSWER_FOR_CHECKING.xlsx
+++ b/server/src/api/INPUT_/NaturaLP_ANSWER_FOR_CHECKING.xlsx
@@ -25,88 +25,91 @@
     <t>Категория</t>
   </si>
   <si>
+    <t>Популярные спортсмены делятся советами о физической активности и питании для поддержания здоровья.</t>
+  </si>
+  <si>
+    <t>Игроки активно делятся своими впечатлениями от недавно вышедших игр и советами для новичков.</t>
+  </si>
+  <si>
     <t>Профессиональные маркетологи делятся советами по увеличению конверсии в онлайн-бизнесе.</t>
   </si>
   <si>
+    <t>Мастерицы делятся идеями для создания уютных декоративных подушек своими руками.</t>
+  </si>
+  <si>
+    <t>Блогер-мотиватор опубликовал новую статью о методах улучшения психологического благополучия.</t>
+  </si>
+  <si>
     <t>Блогер-путешественник поделился впечатлениями о своем последнем путешествии в тропический рай.</t>
   </si>
   <si>
-    <t>Блогер-мотиватор опубликовал новую статью о методах улучшения психологического благополучия.</t>
-  </si>
-  <si>
-    <t>Мастерицы делятся идеями для создания уютных декоративных подушек своими руками.</t>
-  </si>
-  <si>
-    <t>Игроки активно делятся своими впечатлениями от недавно вышедших игр и советами для новичков.</t>
-  </si>
-  <si>
-    <t>Популярные спортсмены делятся советами о физической активности и питании для поддержания здоровья.</t>
+    <t>Известный журналист расследует скандал в правительстве и обещает представить эксклюзивные материалы.</t>
+  </si>
+  <si>
+    <t>Крупная маркетинговая агентство запустила инновационную рекламную кампанию с использованием VR-технологий.</t>
+  </si>
+  <si>
+    <t>Популярный психолог опубликовал книгу о саморазвитии, которая стала бестселлером.</t>
+  </si>
+  <si>
+    <t>Мировые СМИ отмечают увеличение числа подписчиков на новостных платформах во время последних событий.</t>
   </si>
   <si>
     <t>Крупная технологическая компания представила концепт автономного беспилотного автомобиля будущего.</t>
   </si>
   <si>
-    <t>Крупная маркетинговая агентство запустила инновационную рекламную кампанию с использованием VR-технологий.</t>
-  </si>
-  <si>
-    <t>Мировые СМИ отмечают увеличение числа подписчиков на новостных платформах во время последних событий.</t>
+    <t>Крупная авиакомпания объявила о планах по внедрению экологически чистых самолетов в свой парк.</t>
   </si>
   <si>
     <t>Крупное новостное агентство запустило специальный раздел о космических открытиях и миссиях.</t>
   </si>
   <si>
-    <t>Крупная авиакомпания объявила о планах по внедрению экологически чистых самолетов в свой парк.</t>
-  </si>
-  <si>
-    <t>Известный журналист расследует скандал в правительстве и обещает представить эксклюзивные материалы.</t>
-  </si>
-  <si>
     <t>Крупная корпорация представила свою стратегию цифровой трансформации с целью улучшения эффективности бизнеса.</t>
   </si>
   <si>
-    <t>Популярный психолог опубликовал книгу о саморазвитии, которая стала бестселлером.</t>
+    <t>Компания Apple анонсировала новый смартфон с инновационной технологией сканирования радужки глаза.</t>
+  </si>
+  <si>
+    <t>Исследователи создали прорыв в области квантовых компьютеров, что может изменить будущее вычислительной техники.</t>
   </si>
   <si>
     <t>Искусственный интеллект успешно предсказал результаты последних выборов с точностью 95%.</t>
   </si>
   <si>
-    <t>Компания Apple анонсировала новый смартфон с инновационной технологией сканирования радужки глаза.</t>
-  </si>
-  <si>
-    <t>Исследователи создали прорыв в области квантовых компьютеров, что может изменить будущее вычислительной техники.</t>
+    <t>Кризис на рынке акций вызвал беспокойство среди инвесторов, но также создал возможности для долгосрочных инвестиций.</t>
+  </si>
+  <si>
+    <t>Криптовалютные инвестиции привлекают внимание как опытных, так и новичков-инвесторов, предоставляя высокий рост активов.</t>
+  </si>
+  <si>
+    <t>Регуляторы разрабатывают новые правила для регулирования криптовалютных бирж и ICO-проектов.</t>
+  </si>
+  <si>
+    <t>Банк представил новые условия по ипотечным кредитам, что может стимулировать рост рынка недвижимости.</t>
+  </si>
+  <si>
+    <t>Экспорт сельскохозяйственной продукции увеличился благодаря новым торговым соглашениям.</t>
+  </si>
+  <si>
+    <t>Ведущие мировые биржи отметили новый рост цен на нефть, подталкивая акции нефтяных компаний вверх.</t>
   </si>
   <si>
     <t>Инфляция в стране достигла низших значений за последние 10 лет, спровоцировав рост потребительского спроса.</t>
   </si>
   <si>
-    <t>Ведущие мировые биржи отметили новый рост цен на нефть, подталкивая акции нефтяных компаний вверх.</t>
-  </si>
-  <si>
-    <t>Кризис на рынке акций вызвал беспокойство среди инвесторов, но также создал возможности для долгосрочных инвестиций.</t>
-  </si>
-  <si>
-    <t>Регуляторы разрабатывают новые правила для регулирования криптовалютных бирж и ICO-проектов.</t>
-  </si>
-  <si>
-    <t>Экспорт сельскохозяйственной продукции увеличился благодаря новым торговым соглашениям.</t>
-  </si>
-  <si>
-    <t>Банк представил новые условия по ипотечным кредитам, что может стимулировать рост рынка недвижимости.</t>
-  </si>
-  <si>
-    <t>Криптовалютные инвестиции привлекают внимание как опытных, так и новичков-инвесторов, предоставляя высокий рост активов.</t>
+    <t>Стартап, разрабатывающий дронов для доставки еды, привлек новое крупное инвестиционное финансирование.</t>
   </si>
   <si>
     <t>Новый бизнес-инкубатор предоставит стартапам финансовую поддержку и экспертное сопровождение.</t>
   </si>
   <si>
+    <t>Стартап разработал умный городской транспорт, который снижает загрязнение воздуха и уровень пробок.</t>
+  </si>
+  <si>
     <t>Молодой предприниматель запустил успешный онлайн-магазин с экологически чистыми товарами.</t>
   </si>
   <si>
-    <t>Стартап разработал умный городской транспорт, который снижает загрязнение воздуха и уровень пробок.</t>
-  </si>
-  <si>
-    <t>Стартап, разрабатывающий дронов для доставки еды, привлек новое крупное инвестиционное финансирование.</t>
+    <t>Популярные туристические направления восстанавливаются после пандемии, привлекая множество посетителей.</t>
   </si>
   <si>
     <t>Туристическое агентство запустило эксклюзивные путешествия для любителей экстрима и приключений.</t>
@@ -115,55 +118,58 @@
     <t>Горнолыжные курорты собираются к новому сезону, предоставляя туристам широкий спектр развлечений.</t>
   </si>
   <si>
-    <t>Популярные туристические направления восстанавливаются после пандемии, привлекая множество посетителей.</t>
-  </si>
-  <si>
     <t>Компания объявила о запуске программы обучения для предпринимателей и молодых бизнесменов.</t>
   </si>
   <si>
     <t>Рекламные агентства активно исследуют возможности использования искусственного интеллекта для персонализации рекламы.</t>
   </si>
   <si>
+    <t>Психологические консультанты рекомендуют заниматься практикой благодарности для улучшения эмоционального состояния.</t>
+  </si>
+  <si>
     <t>Психологи проводят исследование о влиянии социальных сетей на психическое здоровье подростков.</t>
   </si>
   <si>
     <t>Исследование показало, что медитация и йога помогают снизить уровень стресса и тревожности у большинства людей.</t>
   </si>
   <si>
-    <t>Психологические консультанты рекомендуют заниматься практикой благодарности для улучшения эмоционального состояния.</t>
+    <t>Дизайн-студия разработала инновационное упаковочное решение, снижающее экологическую нагрузку.</t>
+  </si>
+  <si>
+    <t>Города-туристические дестинации представили новые проекты по сохранению культурного наследия.</t>
   </si>
   <si>
     <t>Дизайн-агентство запустило кампанию по переосмыслению бренда крупной корпорации.</t>
   </si>
   <si>
-    <t>Дизайн-студия разработала инновационное упаковочное решение, снижающее экологическую нагрузку.</t>
-  </si>
-  <si>
-    <t>Города-туристические дестинации представили новые проекты по сохранению культурного наследия.</t>
-  </si>
-  <si>
     <t>Кандидаты в президенты представили свои программы на предстоящих выборах, обещая реформы в экономике и образовании.</t>
   </si>
   <si>
+    <t>Парламент принял новый закон о социальных выплатах, который вызвал активные обсуждения в обществе.</t>
+  </si>
+  <si>
+    <t>Лидеры мировых держав провели встречу для обсуждения мер по снижению глобального изменения климата.</t>
+  </si>
+  <si>
+    <t>Мировые лидеры обсудили меры по разрешению конфликта в регионе и поддержке мира.</t>
+  </si>
+  <si>
     <t>Политический аналитик дал свой прогноз на исход предстоящих выборов и их влияние на политическую сцену.</t>
   </si>
   <si>
-    <t>Лидеры мировых держав провели встречу для обсуждения мер по снижению глобального изменения климата.</t>
-  </si>
-  <si>
-    <t>Парламент принял новый закон о социальных выплатах, который вызвал активные обсуждения в обществе.</t>
-  </si>
-  <si>
-    <t>Мировые лидеры обсудили меры по разрешению конфликта в регионе и поддержке мира.</t>
+    <t>Шоу-бизнес обсуждает номинантов на грядущую церемонию вручения премии за выдающиеся достижения в искусстве.</t>
+  </si>
+  <si>
+    <t>Известный художник представил выставку своих новых произведений, вдохновленных природой и мифологией.</t>
+  </si>
+  <si>
+    <t>Фестиваль стрит-фуда привлекает гурманов со всего города, представляя блюда из разных кухонь мира.</t>
   </si>
   <si>
     <t>Комикс-конвент приглашает всех поклонников косплея на выставку в стиле фантастики.</t>
   </si>
   <si>
-    <t>Фестиваль стрит-фуда привлекает гурманов со всего города, представляя блюда из разных кухонь мира.</t>
-  </si>
-  <si>
-    <t>Известный художник представил выставку своих новых произведений, вдохновленных природой и мифологией.</t>
+    <t>Музей современного искусства пригласил зрителей на интерактивную выставку, где можно стать частью произведений искусства.</t>
   </si>
   <si>
     <t>Художники выпустили новую коллекцию ручной росписи на керамике, вдохновленную природой.</t>
@@ -175,85 +181,82 @@
     <t>Балетная труппа впечатлила зрителей новым спектаклем, сочетающим классику и современность.</t>
   </si>
   <si>
-    <t>Музей современного искусства пригласил зрителей на интерактивную выставку, где можно стать частью произведений искусства.</t>
-  </si>
-  <si>
-    <t>Шоу-бизнес обсуждает номинантов на грядущую церемонию вручения премии за выдающиеся достижения в искусстве.</t>
+    <t>Группа правозащитников начала кампанию по борьбе за права меньшинств в обществе.</t>
   </si>
   <si>
     <t>Международный суд рассматривает дело о нарушении прав человека в конфликтной зоне.</t>
   </si>
   <si>
+    <t>Законодатели обсуждают новый проект закона о кибербезопасности и защите данных граждан.</t>
+  </si>
+  <si>
+    <t>Адвокаты предоставили свои комментарии по делу о нарушении авторских прав в музыкальной индустрии.</t>
+  </si>
+  <si>
+    <t>Новая исследовательская статья о влиянии социальных сетей на формирование общественного мнения вызвала обсуждение.</t>
+  </si>
+  <si>
     <t>Верховный суд принял важное решение по делу о защите прав потребителей в интернете.</t>
   </si>
   <si>
-    <t>Законодатели обсуждают новый проект закона о кибербезопасности и защите данных граждан.</t>
-  </si>
-  <si>
-    <t>Группа правозащитников начала кампанию по борьбе за права меньшинств в обществе.</t>
-  </si>
-  <si>
-    <t>Новая исследовательская статья о влиянии социальных сетей на формирование общественного мнения вызвала обсуждение.</t>
-  </si>
-  <si>
-    <t>Адвокаты предоставили свои комментарии по делу о нарушении авторских прав в музыкальной индустрии.</t>
+    <t>Терапевты рассказывают о методах борьбы с посттравматическим стрессом у ветеранов.</t>
+  </si>
+  <si>
+    <t>Команда ученых представила результаты своих исследований в области космической астрофизики.</t>
+  </si>
+  <si>
+    <t>Университет запустил бесплатный онлайн-курс по искусственному интеллекту для всех желающих.</t>
   </si>
   <si>
     <t>Проект по обучению программированию в школах получил государственную поддержку и расширяется на всю страну.</t>
   </si>
   <si>
-    <t>Университет запустил бесплатный онлайн-курс по искусственному интеллекту для всех желающих.</t>
+    <t>Исследователи представили новые методы обучения, улучшающие понимание математики у школьников.</t>
   </si>
   <si>
     <t>Студенты учатся в онлайн-формате, что изменяет традиционный образ образования.</t>
   </si>
   <si>
-    <t>Команда ученых представила результаты своих исследований в области космической астрофизики.</t>
-  </si>
-  <si>
-    <t>Терапевты рассказывают о методах борьбы с посттравматическим стрессом у ветеранов.</t>
-  </si>
-  <si>
-    <t>Исследователи представили новые методы обучения, улучшающие понимание математики у школьников.</t>
+    <t>Спортсмен выразил свою благодарность тренеру и команде за поддержку во время соревнований.</t>
+  </si>
+  <si>
+    <t>Молодые спортсмены побили рекорды в плавании и показали потенциал для будущих Олимпийских игр.</t>
+  </si>
+  <si>
+    <t>Чемпионат мира по футболу завершился с новым чемпионом и неожиданными результатами.</t>
   </si>
   <si>
     <t>Теннисистка вернулась на корт после длительной паузы из-за травмы, вызвав аплодисменты зрителей.</t>
   </si>
   <si>
-    <t>Спортсмен выразил свою благодарность тренеру и команде за поддержку во время соревнований.</t>
-  </si>
-  <si>
-    <t>Чемпионат мира по футболу завершился с новым чемпионом и неожиданными результатами.</t>
-  </si>
-  <si>
-    <t>Молодые спортсмены побили рекорды в плавании и показали потенциал для будущих Олимпийских игр.</t>
+    <t>Дизайнеры работают над созданием виртуальных миров и интерфейсов для расширенной реальности.</t>
+  </si>
+  <si>
+    <t>Успешный ресторанный бренд провел благотворительную акцию, что положительно повлияло на его имидж.</t>
+  </si>
+  <si>
+    <t>Крупный косметический бренд анонсировал сотрудничество с известным визажистом для создания новой линии макияжа.</t>
+  </si>
+  <si>
+    <t>Косметологическая клиника предложила новые процедуры для ухода за кожей с использованием передовых технологий.</t>
   </si>
   <si>
     <t>Дизайнеры представили новую коллекцию осенней одежды с акцентом на экологическую устойчивость.</t>
   </si>
   <si>
-    <t>Успешный ресторанный бренд провел благотворительную акцию, что положительно повлияло на его имидж.</t>
-  </si>
-  <si>
-    <t>Крупный косметический бренд анонсировал сотрудничество с известным визажистом для создания новой линии макияжа.</t>
-  </si>
-  <si>
-    <t>Косметологическая клиника предложила новые процедуры для ухода за кожей с использованием передовых технологий.</t>
+    <t>Мастерица представила свои авторские украшения из натуральных материалов на выставке искусства и ремесел.</t>
+  </si>
+  <si>
+    <t>Мировые модельеры представили новые тренды в мире моды на неделях моды в Париже и Нью-Йорке.</t>
   </si>
   <si>
     <t>Картина художника получила мировое признание и была выставлена на аукционе с высокой оценкой.</t>
   </si>
   <si>
-    <t>Дизайнеры работают над созданием виртуальных миров и интерфейсов для расширенной реальности.</t>
-  </si>
-  <si>
     <t>Мастер-класс по вязанию собрал любителей рукоделия, желающих научиться создавать уникальные вещи.</t>
   </si>
   <si>
-    <t>Мировые модельеры представили новые тренды в мире моды на неделях моды в Париже и Нью-Йорке.</t>
-  </si>
-  <si>
-    <t>Мастерица представила свои авторские украшения из натуральных материалов на выставке искусства и ремесел.</t>
+    <t>Медицинский центр представил новую технологию диагностики и лечения сердечных заболеваний.</t>
   </si>
   <si>
     <t>Врачи рассказывают о важности профилактики и здорового образа жизни для предотвращения хронических заболеваний.</t>
@@ -265,87 +268,84 @@
     <t>Мировые ученые исследуют влияние психического здоровья на общее благополучие и продолжительность жизни.</t>
   </si>
   <si>
-    <t>Медицинский центр представил новую технологию диагностики и лечения сердечных заболеваний.</t>
+    <t>Фотожурналисты документируют важные события и исторические моменты через объектив камеры.</t>
+  </si>
+  <si>
+    <t>Новый круизный лайнер представил маршруты по изучению экзотических островов в Тихом океане.</t>
   </si>
   <si>
     <t>Фотограф опубликовал впечатляющий снимок звездного неба, сделанный в удаленной местности.</t>
   </si>
   <si>
+    <t>Национальный географический журнал представил коллекцию фотографий дикой природы и животных.</t>
+  </si>
+  <si>
     <t>Фотограф-путешественник поделился впечатляющими фотографиями с экспедиции на Антарктиду.</t>
   </si>
   <si>
-    <t>Национальный географический журнал представил коллекцию фотографий дикой природы и животных.</t>
-  </si>
-  <si>
-    <t>Новый круизный лайнер представил маршруты по изучению экзотических островов в Тихом океане.</t>
-  </si>
-  <si>
-    <t>Фотожурналисты документируют важные события и исторические моменты через объектив камеры.</t>
-  </si>
-  <si>
     <t>Фотограф выпустил книгу, собрав в ней свои лучшие работы, сделанные в разных уголках мира.</t>
   </si>
   <si>
     <t>Популярное приложение для здоровья и фитнеса обновило интерфейс и добавило новые функции.</t>
   </si>
   <si>
+    <t>Команда программистов разработала новое приложение для планирования и автоматизации задач в рабочем процессе.</t>
+  </si>
+  <si>
+    <t>Инновационное приложение для обучения иностранным языкам получило множество положительных отзывов от пользователей.</t>
+  </si>
+  <si>
     <t>Разработчики мессенджера выпустили обновление с расширенными возможностями шифрования сообщений.</t>
   </si>
   <si>
-    <t>Инновационное приложение для обучения иностранным языкам получило множество положительных отзывов от пользователей.</t>
-  </si>
-  <si>
-    <t>Команда программистов разработала новое приложение для планирования и автоматизации задач в рабочем процессе.</t>
+    <t>Онлайн-стриминговый сервис представил список ожидаемых фильмов и сериалов на ближайший год.</t>
+  </si>
+  <si>
+    <t>Инфлюэнсеры стали важным каналом для продвижения продуктов и услуг, генерируя миллионы лайков и комментариев.</t>
   </si>
   <si>
     <t>Актриса получила премию за выдающуюся роль в последнем фильме и выразила благодарность своей команде.</t>
   </si>
   <si>
+    <t>Документальный фильм о жизни известной личности вызвал обсуждение и восхищение зрителей.</t>
+  </si>
+  <si>
     <t>Завершились съемки долгожданного блокбастера, который обещает стать хитом кинопроката.</t>
   </si>
   <si>
-    <t>Онлайн-стриминговый сервис представил список ожидаемых фильмов и сериалов на ближайший год.</t>
-  </si>
-  <si>
-    <t>Документальный фильм о жизни известной личности вызвал обсуждение и восхищение зрителей.</t>
-  </si>
-  <si>
-    <t>Инфлюэнсеры стали важным каналом для продвижения продуктов и услуг, генерируя миллионы лайков и комментариев.</t>
+    <t>Фестиваль кино и искусства собрал креативных режиссеров и актеров со всего мира.</t>
+  </si>
+  <si>
+    <t>Мировые звезды музыки поднимают важные социальные вопросы в своих песнях, привлекая внимание общества.</t>
+  </si>
+  <si>
+    <t>Известная рок-группа выпустила новый альбом, который сразу же стал лидером чартов.</t>
+  </si>
+  <si>
+    <t>Швейный кружок организовал благотворительный ярмарку с handmade изделиями для сбора средств на нужды детей.</t>
+  </si>
+  <si>
+    <t>Музыкальная индустрия ожидает выпуска альбома от известной группы, которая вернулась после долгого перерыва.</t>
   </si>
   <si>
     <t>Кинокомпания анонсировала выпуск продолжения популярной комедии, вызвав радостные реакции фанатов.</t>
   </si>
   <si>
-    <t>Известная рок-группа выпустила новый альбом, который сразу же стал лидером чартов.</t>
-  </si>
-  <si>
-    <t>Швейный кружок организовал благотворительный ярмарку с handmade изделиями для сбора средств на нужды детей.</t>
-  </si>
-  <si>
-    <t>Мировые звезды музыки поднимают важные социальные вопросы в своих песнях, привлекая внимание общества.</t>
-  </si>
-  <si>
-    <t>Музыкальная индустрия ожидает выпуска альбома от известной группы, которая вернулась после долгого перерыва.</t>
-  </si>
-  <si>
-    <t>Фестиваль кино и искусства собрал креативных режиссеров и актеров со всего мира.</t>
-  </si>
-  <si>
     <t>Индустрия музыки активно исследует влияние искусственного интеллекта на создание музыки.</t>
   </si>
   <si>
+    <t>Игровая компания представила новый симулятор виртуальной реальности с потрясающей графикой.</t>
+  </si>
+  <si>
+    <t>Ожидается выпуск долгожданной игры с открытым миром, который обещает быть огромным и интересным.</t>
+  </si>
+  <si>
     <t>Игровой турнир собрал лучших киберспортсменов со всего мира для борьбы за призовой фонд.</t>
   </si>
   <si>
     <t>Олимпийские игры привлекли внимание мировых спортсменов и болельщиков, предоставив уникальные спортивные моменты.</t>
   </si>
   <si>
-    <t>Ожидается выпуск долгожданной игры с открытым миром, который обещает быть огромным и интересным.</t>
-  </si>
-  <si>
-    <t>Игровая компания представила новый симулятор виртуальной реальности с потрясающей графикой.</t>
-  </si>
-  <si>
     <t>Известный разработчик анонсировал новую часть популярной игровой франшизы, вызвав ажиотаж среди фанатов.</t>
   </si>
   <si>
@@ -355,25 +355,37 @@
     <t>Повара проводят мастер-классы по приготовлению блюд с использованием местных продуктов.</t>
   </si>
   <si>
+    <t>Популярный шеф-повар представил новое меню в своем ресторане, вдохновленное сезонными продуктами.</t>
+  </si>
+  <si>
     <t>Известный ресторан получил международное признание за свою кулинарную креативность и уникальные блюда.</t>
   </si>
   <si>
-    <t>Популярный шеф-повар представил новое меню в своем ресторане, вдохновленное сезонными продуктами.</t>
+    <t>Известный философ сказал: 'Истинное богатство – это способность быть счастливым с тем, что у тебя есть.'</t>
+  </si>
+  <si>
+    <t>Мудрая цитата: 'Самая большая награда за труд – это не то, что ты заработал, а кто ты стал в процессе.'</t>
+  </si>
+  <si>
+    <t>Мотивационная цитата: 'Путь к успеху начинается с первого шага, и каждый следующий шаг приближает тебя к цели.'</t>
+  </si>
+  <si>
+    <t>Цитата дня: 'Умение радоваться мелочам делает жизнь богаче.'</t>
   </si>
   <si>
     <t>Известный лидер сказал: 'Любовь и сострадание - ключи к гармоничным отношениям и миру в мире.'</t>
   </si>
   <si>
-    <t>Мудрая цитата: 'Самая большая награда за труд – это не то, что ты заработал, а кто ты стал в процессе.'</t>
-  </si>
-  <si>
-    <t>Мотивационная цитата: 'Путь к успеху начинается с первого шага, и каждый следующий шаг приближает тебя к цели.'</t>
-  </si>
-  <si>
-    <t>Известный философ сказал: 'Истинное богатство – это способность быть счастливым с тем, что у тебя есть.'</t>
-  </si>
-  <si>
-    <t>Цитата дня: 'Умение радоваться мелочам делает жизнь богаче.'</t>
+    <t>Эксперты прогнозируют устойчивый рост рынка криптовалют и инвестиций в этот сектор.</t>
+  </si>
+  <si>
+    <t>Эксперты предупреждают о рисках инвестирования в альткоины, призывая осторожность.</t>
+  </si>
+  <si>
+    <t>Инвесторы активно исследуют возможности вложений в зеленые технологии и экологически чистые компании.</t>
+  </si>
+  <si>
+    <t>Крупные финансовые институты увеличивают свои инвестиции в криптовалютные активы.</t>
   </si>
   <si>
     <t>Экономисты анализируют влияние инфляции на покупательскую способность населения и финансовый рынок.</t>
@@ -382,61 +394,49 @@
     <t>Главные новости дня: важные политические решения и международные соглашения.</t>
   </si>
   <si>
-    <t>Инвесторы активно исследуют возможности вложений в зеленые технологии и экологически чистые компании.</t>
-  </si>
-  <si>
-    <t>Эксперты прогнозируют устойчивый рост рынка криптовалют и инвестиций в этот сектор.</t>
-  </si>
-  <si>
-    <t>Эксперты предупреждают о рисках инвестирования в альткоины, призывая осторожность.</t>
-  </si>
-  <si>
     <t>Страны рассматривают варианты создания собственных цифровых валют национальных банков.</t>
   </si>
   <si>
-    <t>Крупные финансовые институты увеличивают свои инвестиции в криптовалютные активы.</t>
+    <t>Звезда кино инвестировала в свой собственный бренд парфюмерии, который стал хитом продаж.</t>
+  </si>
+  <si>
+    <t>Популярная певица готовится к мировому турне, который ожидается как одно из главных музыкальных событий года.</t>
   </si>
   <si>
     <t>Известный блогер проведет онлайн-мастер-класс по созданию стильных образов на осенний сезон.</t>
   </si>
   <si>
-    <t>Популярная певица готовится к мировому турне, который ожидается как одно из главных музыкальных событий года.</t>
+    <t>Знаменитая актриса объявила о своем участии в новом кинопроекте, который вызвал интерес у фанатов.</t>
+  </si>
+  <si>
+    <t>Известный юморист выпустил новый стендап, в котором рассказал о повседневных нелепостях.</t>
+  </si>
+  <si>
+    <t>Молодая певица представила свою дебютную песню, завоевав слушателей своим талантом.</t>
+  </si>
+  <si>
+    <t>Биткоин достиг нового исторического максимума, превысив отметку в $100,000.</t>
+  </si>
+  <si>
+    <t>Популярный музыкальный фестиваль объявил список исполнителей на главной сцене.</t>
+  </si>
+  <si>
+    <t>Комедийный фестиваль представит новую команду юмористов, обещая ночь смеха и веселья.</t>
+  </si>
+  <si>
+    <t>Популярный блогер рассказал о своей новой книге, посвященной приключениям в путешествиях по миру.</t>
+  </si>
+  <si>
+    <t>Известный режиссер анонсировал работу над новым проектом, ориентированным на фанатов научной фантастики.</t>
   </si>
   <si>
     <t>Кулинарный блогер поделился рецептом приготовления популярного десерта, который можно сделать в домашних условиях.</t>
   </si>
   <si>
-    <t>Звезда кино инвестировала в свой собственный бренд парфюмерии, который стал хитом продаж.</t>
-  </si>
-  <si>
-    <t>Комедийный фестиваль представит новую команду юмористов, обещая ночь смеха и веселья.</t>
-  </si>
-  <si>
-    <t>Популярный блогер рассказал о своей новой книге, посвященной приключениям в путешествиях по миру.</t>
-  </si>
-  <si>
     <t>Известный дизайнер представил новую коллекцию мебели, вдохновленную природой.</t>
   </si>
   <si>
-    <t>Знаменитая актриса объявила о своем участии в новом кинопроекте, который вызвал интерес у фанатов.</t>
-  </si>
-  <si>
     <t>Талантливый молодой актер получил приглашение на главную роль в новом голливудском блокбастере.</t>
-  </si>
-  <si>
-    <t>Молодая певица представила свою дебютную песню, завоевав слушателей своим талантом.</t>
-  </si>
-  <si>
-    <t>Известный юморист выпустил новый стендап, в котором рассказал о повседневных нелепостях.</t>
-  </si>
-  <si>
-    <t>Биткоин достиг нового исторического максимума, превысив отметку в $100,000.</t>
-  </si>
-  <si>
-    <t>Популярный музыкальный фестиваль объявил список исполнителей на главной сцене.</t>
-  </si>
-  <si>
-    <t>Известный режиссер анонсировал работу над новым проектом, ориентированным на фанатов научной фантастики.</t>
   </si>
   <si>
     <t>Мировой рекордсмен по головоломкам показал свой новый трюк, оставив зрителей в восхищении.</t>
@@ -898,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -912,7 +912,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -926,7 +926,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -954,7 +954,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -968,7 +968,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -982,7 +982,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -1010,7 +1010,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1024,7 +1024,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1038,7 +1038,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -1052,7 +1052,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1066,7 +1066,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -1080,7 +1080,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1094,7 +1094,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -1108,7 +1108,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -1122,7 +1122,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -1136,7 +1136,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
@@ -1150,7 +1150,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
@@ -1164,7 +1164,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>134</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
@@ -1178,7 +1178,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
@@ -1206,7 +1206,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>132</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
         <v>25</v>
@@ -1220,7 +1220,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>135</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
         <v>26</v>
@@ -1234,7 +1234,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
@@ -1248,7 +1248,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -1276,7 +1276,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
         <v>30</v>
@@ -1290,7 +1290,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
         <v>31</v>
@@ -1304,7 +1304,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
         <v>32</v>
@@ -1318,7 +1318,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
         <v>33</v>
@@ -1360,7 +1360,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
@@ -1374,7 +1374,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
         <v>37</v>
@@ -1388,7 +1388,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
@@ -1402,7 +1402,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
         <v>39</v>
@@ -1416,7 +1416,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
         <v>40</v>
@@ -1430,7 +1430,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
         <v>41</v>
@@ -1458,7 +1458,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
         <v>43</v>
@@ -1486,7 +1486,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
         <v>45</v>
@@ -1500,7 +1500,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
         <v>46</v>
@@ -1514,7 +1514,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="C46" t="s">
         <v>47</v>
@@ -1528,7 +1528,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>118</v>
+        <v>61</v>
       </c>
       <c r="C47" t="s">
         <v>48</v>
@@ -1542,7 +1542,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
         <v>49</v>
@@ -1556,7 +1556,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>128</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
         <v>50</v>
@@ -1570,7 +1570,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
         <v>51</v>
@@ -1584,7 +1584,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
         <v>52</v>
@@ -1598,7 +1598,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C52" t="s">
         <v>53</v>
@@ -1612,7 +1612,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>138</v>
+        <v>64</v>
       </c>
       <c r="C53" t="s">
         <v>54</v>
@@ -1626,7 +1626,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C54" t="s">
         <v>55</v>
@@ -1640,7 +1640,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
         <v>56</v>
@@ -1668,7 +1668,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C57" t="s">
         <v>58</v>
@@ -1696,7 +1696,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C59" t="s">
         <v>60</v>
@@ -1710,7 +1710,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="C60" t="s">
         <v>61</v>
@@ -1724,7 +1724,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C61" t="s">
         <v>62</v>
@@ -1738,7 +1738,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C62" t="s">
         <v>63</v>
@@ -1752,7 +1752,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C63" t="s">
         <v>64</v>
@@ -1766,7 +1766,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="C64" t="s">
         <v>65</v>
@@ -1780,7 +1780,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C65" t="s">
         <v>66</v>
@@ -1794,7 +1794,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C66" t="s">
         <v>67</v>
@@ -1808,7 +1808,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C67" t="s">
         <v>68</v>
@@ -1836,7 +1836,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C69" t="s">
         <v>70</v>
@@ -1850,7 +1850,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C70" t="s">
         <v>71</v>
@@ -1906,7 +1906,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C74" t="s">
         <v>75</v>
@@ -1920,7 +1920,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C75" t="s">
         <v>76</v>
@@ -1934,7 +1934,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="C76" t="s">
         <v>77</v>
@@ -1948,7 +1948,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C77" t="s">
         <v>78</v>
@@ -1962,7 +1962,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C78" t="s">
         <v>79</v>
@@ -1976,7 +1976,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C79" t="s">
         <v>80</v>
@@ -1990,7 +1990,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C80" t="s">
         <v>81</v>
@@ -2004,7 +2004,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C81" t="s">
         <v>82</v>
@@ -2018,7 +2018,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C82" t="s">
         <v>83</v>
@@ -2032,7 +2032,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C83" t="s">
         <v>84</v>
@@ -2046,7 +2046,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="C84" t="s">
         <v>85</v>
@@ -2060,7 +2060,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C85" t="s">
         <v>86</v>
@@ -2074,7 +2074,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="C86" t="s">
         <v>87</v>
@@ -2088,7 +2088,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C87" t="s">
         <v>88</v>
@@ -2130,7 +2130,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C90" t="s">
         <v>91</v>
@@ -2158,7 +2158,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C92" t="s">
         <v>93</v>
@@ -2172,7 +2172,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="C93" t="s">
         <v>94</v>
@@ -2186,7 +2186,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="C94" t="s">
         <v>95</v>
@@ -2200,7 +2200,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="C95" t="s">
         <v>96</v>
@@ -2228,7 +2228,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="C97" t="s">
         <v>98</v>
@@ -2242,7 +2242,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="C98" t="s">
         <v>99</v>
@@ -2256,7 +2256,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C99" t="s">
         <v>100</v>
@@ -2270,7 +2270,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C100" t="s">
         <v>101</v>
@@ -2284,7 +2284,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="C101" t="s">
         <v>102</v>
@@ -2312,7 +2312,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="C103" t="s">
         <v>104</v>
@@ -2340,7 +2340,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C105" t="s">
         <v>106</v>
@@ -2354,7 +2354,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="C106" t="s">
         <v>107</v>
@@ -2368,7 +2368,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C107" t="s">
         <v>108</v>
@@ -2382,7 +2382,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="C108" t="s">
         <v>109</v>
@@ -2438,7 +2438,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C112" t="s">
         <v>113</v>
@@ -2452,7 +2452,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C113" t="s">
         <v>114</v>
@@ -2466,7 +2466,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C114" t="s">
         <v>115</v>
@@ -2508,7 +2508,7 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C117" t="s">
         <v>118</v>
@@ -2522,7 +2522,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C118" t="s">
         <v>119</v>
@@ -2536,7 +2536,7 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>133</v>
+        <v>25</v>
       </c>
       <c r="C119" t="s">
         <v>120</v>
@@ -2550,7 +2550,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C120" t="s">
         <v>121</v>
@@ -2578,7 +2578,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C122" t="s">
         <v>123</v>
@@ -2592,7 +2592,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="C123" t="s">
         <v>124</v>
@@ -2606,7 +2606,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C124" t="s">
         <v>125</v>
@@ -2620,7 +2620,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C125" t="s">
         <v>126</v>
@@ -2634,7 +2634,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="C126" t="s">
         <v>127</v>
@@ -2662,7 +2662,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="C128" t="s">
         <v>129</v>
@@ -2676,7 +2676,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="C129" t="s">
         <v>130</v>
@@ -2690,7 +2690,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C130" t="s">
         <v>131</v>
@@ -2704,7 +2704,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="C131" t="s">
         <v>132</v>
@@ -2718,7 +2718,7 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C132" t="s">
         <v>133</v>
@@ -2732,7 +2732,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="C133" t="s">
         <v>134</v>
@@ -2746,7 +2746,7 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>139</v>
+        <v>12</v>
       </c>
       <c r="C134" t="s">
         <v>135</v>
@@ -2760,7 +2760,7 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="C135" t="s">
         <v>136</v>
@@ -2774,7 +2774,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="C136" t="s">
         <v>137</v>
@@ -2788,7 +2788,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>31</v>
+        <v>117</v>
       </c>
       <c r="C137" t="s">
         <v>138</v>
@@ -2802,7 +2802,7 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="C138" t="s">
         <v>139</v>
@@ -2816,7 +2816,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="C139" t="s">
         <v>140</v>

</xml_diff>